<commit_message>
Adding experiments on potential radius=5
</commit_message>
<xml_diff>
--- a/MyProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
+++ b/MyProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\MyProject\Dataset Reports\Dataset-GurunagSai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0050B3-1162-4D86-8819-6A504B90A5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED88C105-7200-4B44-A07F-95DC42673EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="2145" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="168">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>Global Inhibition</t>
-  </si>
-  <si>
-    <t>ColumnDimensions</t>
-  </si>
-  <si>
-    <t>InputDimensions</t>
   </si>
   <si>
     <t>64x64</t>
@@ -312,6 +306,339 @@
   </si>
   <si>
     <t>Experiment output (Github URL-https://github.com/GurunagSai/neocortexapi-classification/tree/main/MyProject/Dataset%20Reports/Dataset-GurunagSai/OutputFolder)</t>
+  </si>
+  <si>
+    <t>output-36</t>
+  </si>
+  <si>
+    <t>output-37</t>
+  </si>
+  <si>
+    <t>output-38</t>
+  </si>
+  <si>
+    <t>output-39</t>
+  </si>
+  <si>
+    <t>output-40</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 110</t>
+  </si>
+  <si>
+    <t>proper output but
+variance between max and min for both micro and macro corelation are high</t>
+  </si>
+  <si>
+    <t>proper output but the variance is high
+the micro correlation is 85-65% and macro is 64-34%</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 300</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 700</t>
+  </si>
+  <si>
+    <t>output-41</t>
+  </si>
+  <si>
+    <t>output-42</t>
+  </si>
+  <si>
+    <t>output-43</t>
+  </si>
+  <si>
+    <t>output-44</t>
+  </si>
+  <si>
+    <t>output-45</t>
+  </si>
+  <si>
+    <t>output-46</t>
+  </si>
+  <si>
+    <t>output-47</t>
+  </si>
+  <si>
+    <t>output-48</t>
+  </si>
+  <si>
+    <t>output-49</t>
+  </si>
+  <si>
+    <t>output-50</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 900</t>
+  </si>
+  <si>
+    <t>Both the micro and macro correlation are high but variance is less(90's-75's% for both)</t>
+  </si>
+  <si>
+    <t>Both macro(96-94) and micro(100-96) corelation are higher</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 990</t>
+  </si>
+  <si>
+    <t>Both macro(99-99) and micro(100-99) corelation are higher</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 100</t>
+  </si>
+  <si>
+    <t>circle - rectangle macro is high(85)
+micro(95-70) and macro (85-26)</t>
+  </si>
+  <si>
+    <t>circle - rectangle macro is high(87)
+micro(98-89) and macro (87-51)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 512</t>
+  </si>
+  <si>
+    <t>macro corelation is higher for cirlce-rectangle
+micro (96-83) and macro (86-65)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 716</t>
+  </si>
+  <si>
+    <t>Both macro(94-85) and micro(100-94) corelation are higher</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 921</t>
+  </si>
+  <si>
+    <t>Both macro(100-98) and micro(100-97) corelation are higher</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 134</t>
+  </si>
+  <si>
+    <t>The variance in micro corelation is more
+micro(85-40) and macro(52-17)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 422</t>
+  </si>
+  <si>
+    <t>30
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>valid output
+micro(92-75) and macro(68-45)</t>
+  </si>
+  <si>
+    <t>output-51</t>
+  </si>
+  <si>
+    <t>output-52</t>
+  </si>
+  <si>
+    <t>output-53</t>
+  </si>
+  <si>
+    <t>output-54</t>
+  </si>
+  <si>
+    <t>output-55</t>
+  </si>
+  <si>
+    <t>circle0__circle1
+input sim:82.71%</t>
+  </si>
+  <si>
+    <t>rectangle0_rectangle_1
+input sim: 90.9%</t>
+  </si>
+  <si>
+    <t>triangle0__triangle1
+input sim: 81.87%</t>
+  </si>
+  <si>
+    <t>image1 vs image2 sdr corelations in %</t>
+  </si>
+  <si>
+    <t>InputDimensions
+(pixel x pixel)</t>
+  </si>
+  <si>
+    <t>ColumnDimensions
+(2D topology)</t>
+  </si>
+  <si>
+    <t>50
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 750</t>
+  </si>
+  <si>
+    <t>macro correlation is high
+macro(88-79) and micro(96-86)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80
+inh radius: 4 </t>
+  </si>
+  <si>
+    <t>macro correlation is high
+macro(87-78) and micro(96-86)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100
+inh radius:4 </t>
+  </si>
+  <si>
+    <t>10
+inh radius:4</t>
+  </si>
+  <si>
+    <t>20
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>40
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>output-56</t>
+  </si>
+  <si>
+    <t>output-57</t>
+  </si>
+  <si>
+    <t>output-58</t>
+  </si>
+  <si>
+    <t>output-59</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 250</t>
+  </si>
+  <si>
+    <t>The variance in micro corelation is more
+micro(87-61) and macro(64-29)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 720</t>
+  </si>
+  <si>
+    <t>macro correlation is high
+micro(95-84) and macro(87-72)</t>
+  </si>
+  <si>
+    <t>35
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>output-60</t>
+  </si>
+  <si>
+    <t>10
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 10</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(90-10) and macro (10-0)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 600</t>
+  </si>
+  <si>
+    <t>macro is high
+micro(94-79) and macro(78-53)</t>
+  </si>
+  <si>
+    <t>20
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 20</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(95-35) and macro (40-0)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 30</t>
+  </si>
+  <si>
+    <t>30
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(96-53) and macro (54-0)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 40</t>
+  </si>
+  <si>
+    <t>40
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(95-60) and macro (67.5-0)</t>
+  </si>
+  <si>
+    <t>50
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>80
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>100
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 50</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(90-60) and macro (72-0)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 80</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(93-56) and macro (77-16)</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(96-70) and macro (87-24)</t>
   </si>
 </sst>
 </file>
@@ -349,7 +676,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -398,11 +725,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,6 +791,27 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -709,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="J55" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,15 +1106,18 @@
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="17" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="70.140625" customWidth="1"/>
     <col min="9" max="9" width="71.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="10" width="18.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -740,13 +1128,18 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -757,19 +1150,28 @@
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
+      <c r="F2" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -782,23 +1184,23 @@
       <c r="D3" s="2">
         <v>0.1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="17">
         <v>-1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -811,23 +1213,23 @@
       <c r="D4" s="2">
         <v>0.3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="17">
         <v>-1</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -840,23 +1242,23 @@
       <c r="D5" s="2">
         <v>0.5</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="17">
         <v>-1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -869,23 +1271,23 @@
       <c r="D6" s="2">
         <v>0.7</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="17">
         <v>-1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -898,23 +1300,23 @@
       <c r="D7" s="2">
         <v>0.9</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="17">
         <v>-1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -927,23 +1329,23 @@
       <c r="D8" s="2">
         <v>0.1</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="17">
         <v>-1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -956,23 +1358,23 @@
       <c r="D9" s="2">
         <v>0.3</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="17">
         <v>-1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -985,23 +1387,23 @@
       <c r="D10" s="2">
         <v>0.5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="17">
         <v>-1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1014,23 +1416,23 @@
       <c r="D11" s="2">
         <v>0.7</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="17">
         <v>-1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1043,23 +1445,23 @@
       <c r="D12" s="2">
         <v>0.9</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="17">
         <v>-1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1072,23 +1474,23 @@
       <c r="D13" s="2">
         <v>0.1</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="17">
         <v>-1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1101,23 +1503,23 @@
       <c r="D14" s="2">
         <v>0.3</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="17">
         <v>-1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1130,23 +1532,23 @@
       <c r="D15" s="2">
         <v>0.5</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="17">
         <v>-1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1159,20 +1561,20 @@
       <c r="D16" s="2">
         <v>0.7</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="17">
         <v>-1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1188,20 +1590,20 @@
       <c r="D17" s="2">
         <v>0.9</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="17">
         <v>-1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1217,20 +1619,20 @@
       <c r="D18" s="2">
         <v>0.1</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="17">
         <v>-1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1246,20 +1648,20 @@
       <c r="D19" s="2">
         <v>0.3</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="17">
         <v>-1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1275,20 +1677,20 @@
       <c r="D20" s="2">
         <v>0.5</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="17">
         <v>-1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1304,20 +1706,20 @@
       <c r="D21" s="2">
         <v>0.7</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="17">
         <v>-1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1333,20 +1735,20 @@
       <c r="D22" s="2">
         <v>0.9</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="17">
         <v>-1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1362,20 +1764,20 @@
       <c r="D23" s="2">
         <v>0.15</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="17">
         <v>-1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1391,20 +1793,20 @@
       <c r="D24" s="2">
         <v>0.7</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="17">
         <v>-1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1420,20 +1822,20 @@
       <c r="D25" s="2">
         <v>0.5</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="17">
         <v>-1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1449,20 +1851,20 @@
       <c r="D26" s="2">
         <v>0.3</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="17">
         <v>-1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1478,20 +1880,20 @@
       <c r="D27" s="2">
         <v>-1</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="17">
         <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1507,20 +1909,20 @@
       <c r="D28" s="2">
         <v>-1</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="17">
         <v>20</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="I28" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1536,20 +1938,20 @@
       <c r="D29" s="2">
         <v>-1</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="17">
         <v>50</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="I29" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,20 +1967,20 @@
       <c r="D30" s="2">
         <v>-1</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="17">
         <v>100</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1594,20 +1996,20 @@
       <c r="D31" s="2">
         <v>-1</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="17">
         <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1623,23 +2025,23 @@
       <c r="D32" s="2">
         <v>-1</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="17">
         <v>50</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -1652,23 +2054,23 @@
       <c r="D33" s="2">
         <v>-1</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="17">
         <v>100</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -1681,23 +2083,23 @@
       <c r="D34" s="2">
         <v>-1</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="17">
         <v>100</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -1710,23 +2112,23 @@
       <c r="D35" s="2">
         <v>0.1</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="17">
         <v>-1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -1739,23 +2141,23 @@
       <c r="D36" s="2">
         <v>0.2</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="17">
         <v>-1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -1768,28 +2170,979 @@
       <c r="D37" s="2">
         <v>0.15</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="17">
         <v>-1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>5</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E38" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J38" s="2">
+        <v>72.069999999999993</v>
+      </c>
+      <c r="K38" s="2">
+        <v>82.05</v>
+      </c>
+      <c r="L38" s="2">
+        <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>5</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E39" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J39" s="2">
+        <v>82.46</v>
+      </c>
+      <c r="K39" s="2">
+        <v>86.22</v>
+      </c>
+      <c r="L39" s="2">
+        <v>77.83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="2">
+        <v>94.06</v>
+      </c>
+      <c r="K40" s="2">
+        <v>97.14</v>
+      </c>
+      <c r="L40" s="2">
+        <v>95.34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2">
+        <v>5</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E41" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="2">
+        <v>97.25</v>
+      </c>
+      <c r="K41" s="2">
+        <v>98.6</v>
+      </c>
+      <c r="L41" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E42" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J42" s="2">
+        <v>99.49</v>
+      </c>
+      <c r="K42" s="2">
+        <v>100</v>
+      </c>
+      <c r="L42" s="2">
+        <v>99.79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E43" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J43" s="2">
+        <v>95.09</v>
+      </c>
+      <c r="K43" s="2">
+        <v>94.11</v>
+      </c>
+      <c r="L43" s="2">
+        <v>87.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
+        <v>5</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E44" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J44" s="2">
+        <v>97.39</v>
+      </c>
+      <c r="K44" s="2">
+        <v>97.71</v>
+      </c>
+      <c r="L44" s="2">
+        <v>92.18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E45" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J45" s="2">
+        <v>93.35</v>
+      </c>
+      <c r="K45" s="2">
+        <v>98.24</v>
+      </c>
+      <c r="L45" s="2">
+        <v>91.01</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2">
+        <v>5</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E46" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J46" s="2">
+        <v>96.78</v>
+      </c>
+      <c r="K46" s="2">
+        <v>98.74</v>
+      </c>
+      <c r="L46" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2">
+        <v>5</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E47" s="17">
+        <v>-1</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J47" s="2">
+        <v>100</v>
+      </c>
+      <c r="K47" s="2">
+        <v>99.67</v>
+      </c>
+      <c r="L47" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2">
+        <v>5</v>
+      </c>
+      <c r="D48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J48" s="2">
+        <v>76.64</v>
+      </c>
+      <c r="K48" s="2">
+        <v>81.63</v>
+      </c>
+      <c r="L48" s="2">
+        <v>78.010000000000005</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" s="2">
+        <v>5</v>
+      </c>
+      <c r="D49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J49" s="2">
+        <v>84.83</v>
+      </c>
+      <c r="K49" s="2">
+        <v>91.51</v>
+      </c>
+      <c r="L49" s="2">
+        <v>81.67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50" s="2">
+        <v>5</v>
+      </c>
+      <c r="D50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J50" s="2">
+        <v>93.9</v>
+      </c>
+      <c r="K50" s="2">
+        <v>96.2</v>
+      </c>
+      <c r="L50" s="2">
+        <v>95.48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" s="2">
+        <v>5</v>
+      </c>
+      <c r="D51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J51" s="2">
+        <v>93.79</v>
+      </c>
+      <c r="K51" s="2">
+        <v>96.5</v>
+      </c>
+      <c r="L51" s="2">
+        <v>95.72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52" s="2">
+        <v>5</v>
+      </c>
+      <c r="D52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J52" s="2">
+        <v>93.79</v>
+      </c>
+      <c r="K52" s="2">
+        <v>96.76</v>
+      </c>
+      <c r="L52" s="2">
+        <v>95.73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" s="2">
+        <v>5</v>
+      </c>
+      <c r="D53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J53" s="2">
+        <v>85.76</v>
+      </c>
+      <c r="K53" s="2">
+        <v>85.61</v>
+      </c>
+      <c r="L53" s="2">
+        <v>78.040000000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" s="2">
+        <v>5</v>
+      </c>
+      <c r="D54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J54" s="2">
+        <v>93.38</v>
+      </c>
+      <c r="K54" s="2">
+        <v>94.04</v>
+      </c>
+      <c r="L54" s="2">
+        <v>93.46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="2">
+        <v>5</v>
+      </c>
+      <c r="D55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="2">
+        <v>87.21</v>
+      </c>
+      <c r="K55" s="2">
+        <v>92.9</v>
+      </c>
+      <c r="L55" s="2">
+        <v>85.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J56" s="2">
+        <v>80</v>
+      </c>
+      <c r="K56" s="2">
+        <v>40</v>
+      </c>
+      <c r="L56" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
+        <v>5</v>
+      </c>
+      <c r="D57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J57" s="2">
+        <v>85</v>
+      </c>
+      <c r="K57" s="2">
+        <v>70</v>
+      </c>
+      <c r="L57" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2">
+        <v>5</v>
+      </c>
+      <c r="D58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J58" s="2">
+        <v>83.33</v>
+      </c>
+      <c r="K58" s="2">
+        <v>80</v>
+      </c>
+      <c r="L58" s="2">
+        <v>53.33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J59" s="2">
+        <v>85</v>
+      </c>
+      <c r="K59" s="2">
+        <v>85</v>
+      </c>
+      <c r="L59" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2">
+        <v>5</v>
+      </c>
+      <c r="D60" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J60" s="2">
+        <v>84</v>
+      </c>
+      <c r="K60" s="2">
+        <v>88</v>
+      </c>
+      <c r="L60" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2">
+        <v>5</v>
+      </c>
+      <c r="D61" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J61" s="2">
+        <v>91.25</v>
+      </c>
+      <c r="K61" s="2">
+        <v>92.5</v>
+      </c>
+      <c r="L61" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2">
+        <v>5</v>
+      </c>
+      <c r="D62" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J62" s="2">
+        <v>95</v>
+      </c>
+      <c r="K62" s="2">
+        <v>96</v>
+      </c>
+      <c r="L62" s="2">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>